<commit_message>
Get ready to rebrand
</commit_message>
<xml_diff>
--- a/Datasets/Biomarker Data.xlsx
+++ b/Datasets/Biomarker Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dalla\Box\ADNI\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11474C9E-5175-4B69-8839-8CC0C9AD753A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81C9FF8-E1CD-41FB-8ABD-C8FE35C1CF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4758667A-B518-4719-9E7D-6B95FB46E12C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
   <si>
     <t>Variable</t>
   </si>
@@ -122,9 +122,6 @@
     <t>https://ida.loni.usc.edu/download/files/study/0ad02a84-4c30-4b49-a1a4-3ec9e48ac448/file/adni/ADNI_ADASDCB.pdf</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>UPENNPLASMA</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>AB42</t>
   </si>
   <si>
-    <t>pg/mL</t>
-  </si>
-  <si>
     <t>Abeta1-40 result in plasma</t>
   </si>
   <si>
@@ -152,24 +146,15 @@
     <t>Source Table</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>See "ADNI_Biomarker_Methods_Statistical_Analyses_Dec2023.docx" for info on Z-score calculations</t>
   </si>
   <si>
-    <t>ADSP_PHC_CSF_Dec2023</t>
-  </si>
-  <si>
     <t>AB42_RAW</t>
   </si>
   <si>
     <t>Raw AB42 biomarker levels</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>PHC_AB42</t>
   </si>
   <si>
@@ -198,6 +183,69 @@
   </si>
   <si>
     <t>Harmonized biomarker pTau Z-score (derived - see METHODS)</t>
+  </si>
+  <si>
+    <t>SELKOELAB_OAB</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>Mean amount of A-Beta Oligomer</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>Coefficient of Variation</t>
+  </si>
+  <si>
+    <t>ADSP_PHC_CSF</t>
+  </si>
+  <si>
+    <t>UPENNBIOMK_MASTER</t>
+  </si>
+  <si>
+    <t>ABETA</t>
+  </si>
+  <si>
+    <t>TAU</t>
+  </si>
+  <si>
+    <t>PTAU</t>
+  </si>
+  <si>
+    <t>ABETA_RAW</t>
+  </si>
+  <si>
+    <t>TAU_RAW</t>
+  </si>
+  <si>
+    <t>PTAU_RAW</t>
+  </si>
+  <si>
+    <t>Normalized TAU in CSF</t>
+  </si>
+  <si>
+    <t>Raw tau in CSF</t>
+  </si>
+  <si>
+    <t>Raw ptau (181) beta in CSF</t>
+  </si>
+  <si>
+    <t>Raw amyloid beta (1-42) in CSF</t>
+  </si>
+  <si>
+    <t>Normalized Amyloid Beta (1-42) in CSF</t>
+  </si>
+  <si>
+    <t>Normalized PTAU (181) in CSF</t>
   </si>
 </sst>
 </file>
@@ -583,29 +631,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C848FCB-89CD-4AA6-850D-A615F31C9399}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -621,9 +669,6 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
       <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
@@ -645,9 +690,6 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
@@ -664,9 +706,6 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
@@ -683,9 +722,6 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -700,9 +736,6 @@
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -717,9 +750,6 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
       <c r="G7" t="s">
         <v>26</v>
       </c>
@@ -740,9 +770,6 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -757,9 +784,6 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -774,9 +798,6 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -791,169 +812,265 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
-        <v>32</v>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="G16" t="s">
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="C26" t="s">
         <v>40</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
         <v>41</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
         <v>42</v>
       </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
         <v>44</v>
       </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
         <v>50</v>
       </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
         <v>51</v>
       </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
         <v>52</v>
       </c>
-      <c r="D22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" t="s">
-        <v>28</v>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>